<commit_message>
added files for revision
</commit_message>
<xml_diff>
--- a/notebooks/Feature-description_DHa.xlsx
+++ b/notebooks/Feature-description_DHa.xlsx
@@ -1,15 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="29005"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="10523"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/mk/docker-cinc2017/notebooks/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/mk/ecg-classification/notebooks/"/>
     </mc:Choice>
   </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="10_ncr:8100000_{10F0F53C-9941-0D44-93DD-320F584A2273}" xr6:coauthVersionLast="33" xr6:coauthVersionMax="33" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="460" windowWidth="38400" windowHeight="21140" tabRatio="500"/>
+    <workbookView xWindow="0" yWindow="460" windowWidth="38400" windowHeight="21140" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -17,7 +18,7 @@
   <definedNames>
     <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Sheet1!$C$1:$C$387</definedName>
   </definedNames>
-  <calcPr calcId="150001" concurrentCalc="0"/>
+  <calcPr calcId="150001"/>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{79F54976-1DA5-4618-B147-4CDE4B953A38}">
       <x14:workbookPr defaultImageDpi="32767"/>
@@ -2378,7 +2379,7 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="0.00000"/>
   </numFmts>
@@ -2790,11 +2791,11 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:F387"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="180" zoomScaleNormal="180" workbookViewId="0">
-      <selection activeCell="D10" sqref="D10"/>
+    <sheetView tabSelected="1" topLeftCell="D1" zoomScale="180" zoomScaleNormal="180" workbookViewId="0">
+      <selection activeCell="D8" sqref="D8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14" x14ac:dyDescent="0.2"/>

</xml_diff>